<commit_message>
Edit and Delete Functionality
</commit_message>
<xml_diff>
--- a/data/members.xlsx
+++ b/data/members.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,7 +498,7 @@
         <v>54.8</v>
       </c>
       <c r="F2" t="n">
-        <v>5.7</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -509,28 +509,28 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Ahmed</t>
+          <t>hassan</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Lahore</t>
+          <t>haidrabad</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Premium</t>
+          <t>Luxury</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="F3" t="n">
-        <v>5.5</v>
+        <v>6.1</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -545,28 +545,28 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>hassan</t>
+          <t>Salm</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>haidrabad</t>
+          <t>khi</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Luxury</t>
+          <t>Economy</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="F4" t="n">
-        <v>6.1</v>
+        <v>5.3</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -581,28 +581,28 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Salm</t>
+          <t>Ali</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>khi</t>
+          <t>Islamabad</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Economy</t>
+          <t>Luxury</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="F5" t="n">
-        <v>5.3</v>
+        <v>5.7</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -610,42 +610,6 @@
         </is>
       </c>
       <c r="H5" t="inlineStr">
-        <is>
-          <t>Paid</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Ali</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Islamabad</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Luxury</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>65</v>
-      </c>
-      <c r="F6" t="n">
-        <v>5.7</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>2025-03-05</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
         <is>
           <t>Paid</t>
         </is>

</xml_diff>

<commit_message>
finally everything correctly configured
</commit_message>
<xml_diff>
--- a/data/members.xlsx
+++ b/data/members.xlsx
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="F2" t="n">
         <v>5.4</v>
@@ -567,11 +567,7 @@
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>2025-03-05</t>
-        </is>
-      </c>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
@@ -582,20 +578,14 @@
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>pregnant</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>u</t>
-        </is>
-      </c>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>3</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -604,7 +594,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>kalam</t>
+          <t>jhoopri</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -625,14 +615,14 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Paid</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-03-01</t>
+          <t>2025-03-03</t>
         </is>
       </c>
       <c r="L3" t="inlineStr"/>
@@ -647,7 +637,7 @@
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr">
         <is>
-          <t>strong AF</t>
+          <t>strong</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">

</xml_diff>

<commit_message>
remaing days column added
</commit_message>
<xml_diff>
--- a/data/members.xlsx
+++ b/data/members.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hassaan\Documents\everything\project\New folder\gym_management\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB0CA20-240D-454A-BB8F-EDB0A381B9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>member_id</t>
   </si>
@@ -68,13 +62,46 @@
   </si>
   <si>
     <t>height</t>
+  </si>
+  <si>
+    <t>1001</t>
+  </si>
+  <si>
+    <t>Abdullah</t>
+  </si>
+  <si>
+    <t>Karachi</t>
+  </si>
+  <si>
+    <t>2025-02-23</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Saboor</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>31-03-2025</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Paid</t>
+  </si>
+  <si>
+    <t>Strong</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,7 +112,10 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -134,14 +164,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -429,19 +451,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="A2:Q7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="10" max="10" width="12.81640625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,7 +508,54 @@
         <v>15</v>
       </c>
     </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>3452820243</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2">
+        <v>3452949573</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2">
+        <v>70</v>
+      </c>
+      <c r="P2">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>